<commit_message>
sampling added (based on seasons)
</commit_message>
<xml_diff>
--- a/data/table_sample_stats.xlsx
+++ b/data/table_sample_stats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20366"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20372"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barth\Desktop\Projekte\GFZ\Shany\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barth\Desktop\Projekte\GFZ\Shany\git\ReefBuilderMicrobiome\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811D3066-2709-43DA-A8AD-FBEF998F3973}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3670BA-DD01-46F9-9582-683230495ECA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24375" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="table_sample_stats" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">table_sample_stats!$A$2:$M$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">table_sample_stats!$A$2:$N$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="91">
   <si>
     <t>input</t>
   </si>
@@ -287,6 +287,15 @@
   </si>
   <si>
     <t>Season</t>
+  </si>
+  <si>
+    <t>Sampling</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
   </si>
 </sst>
 </file>
@@ -1260,10 +1269,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1271,7 +1280,7 @@
     <col min="7" max="7" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>78</v>
       </c>
@@ -1282,7 +1291,7 @@
       <c r="F1" s="12"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1311,22 +1320,25 @@
         <v>87</v>
       </c>
       <c r="J2" t="s">
+        <v>88</v>
+      </c>
+      <c r="K2" t="s">
         <v>81</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>80</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>73</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>77</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>44133</v>
       </c>
@@ -1355,20 +1367,23 @@
         <v>79</v>
       </c>
       <c r="J3" t="s">
+        <v>89</v>
+      </c>
+      <c r="K3" t="s">
         <v>82</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>84</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <f>F3/A3</f>
         <v>0.51834228355199052</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>47933</v>
       </c>
@@ -1397,17 +1412,20 @@
         <v>79</v>
       </c>
       <c r="J4" t="s">
+        <v>89</v>
+      </c>
+      <c r="K4" t="s">
         <v>82</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>84</v>
       </c>
-      <c r="L4">
-        <f t="shared" ref="L4:L40" si="0">F4/A4</f>
+      <c r="M4">
+        <f t="shared" ref="M4:M40" si="0">F4/A4</f>
         <v>0.85947051092149462</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>7320</v>
       </c>
@@ -1436,20 +1454,23 @@
         <v>79</v>
       </c>
       <c r="J5" t="s">
+        <v>89</v>
+      </c>
+      <c r="K5" t="s">
         <v>83</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>84</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <f t="shared" si="0"/>
         <v>0.43715846994535518</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>12758</v>
       </c>
@@ -1478,17 +1499,20 @@
         <v>79</v>
       </c>
       <c r="J6" t="s">
+        <v>89</v>
+      </c>
+      <c r="K6" t="s">
         <v>83</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>84</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <f t="shared" si="0"/>
         <v>0.85852014422323253</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>8777</v>
       </c>
@@ -1517,20 +1541,23 @@
         <v>79</v>
       </c>
       <c r="J7" t="s">
+        <v>89</v>
+      </c>
+      <c r="K7" t="s">
         <v>83</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>84</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <f t="shared" si="0"/>
         <v>0.46257263301811552</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>23940</v>
       </c>
@@ -1559,17 +1586,20 @@
         <v>79</v>
       </c>
       <c r="J8" t="s">
+        <v>89</v>
+      </c>
+      <c r="K8" t="s">
         <v>83</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>84</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <f t="shared" si="0"/>
         <v>0.88700918964076858</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>39049</v>
       </c>
@@ -1598,20 +1628,23 @@
         <v>79</v>
       </c>
       <c r="J9" t="s">
+        <v>89</v>
+      </c>
+      <c r="K9" t="s">
         <v>83</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>84</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <f t="shared" si="0"/>
         <v>0.50034571948065254</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>38297</v>
       </c>
@@ -1640,17 +1673,20 @@
         <v>79</v>
       </c>
       <c r="J10" t="s">
+        <v>89</v>
+      </c>
+      <c r="K10" t="s">
         <v>83</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>84</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <f t="shared" si="0"/>
         <v>0.83925633861660187</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>52174</v>
       </c>
@@ -1679,20 +1715,23 @@
         <v>79</v>
       </c>
       <c r="J11" t="s">
+        <v>89</v>
+      </c>
+      <c r="K11" t="s">
         <v>83</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>84</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <f t="shared" si="0"/>
         <v>0.54057576570705712</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>52619</v>
       </c>
@@ -1721,17 +1760,20 @@
         <v>79</v>
       </c>
       <c r="J12" t="s">
+        <v>89</v>
+      </c>
+      <c r="K12" t="s">
         <v>83</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>84</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <f t="shared" si="0"/>
         <v>0.9210361276345046</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>8145</v>
       </c>
@@ -1760,20 +1802,23 @@
         <v>79</v>
       </c>
       <c r="J13" t="s">
+        <v>89</v>
+      </c>
+      <c r="K13" t="s">
         <v>83</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>84</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <f t="shared" si="0"/>
         <v>0.4567219152854512</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>7040</v>
       </c>
@@ -1802,17 +1847,20 @@
         <v>79</v>
       </c>
       <c r="J14" t="s">
+        <v>89</v>
+      </c>
+      <c r="K14" t="s">
         <v>83</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>84</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <f t="shared" si="0"/>
         <v>0.85184659090909087</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>7880</v>
       </c>
@@ -1841,20 +1889,23 @@
         <v>79</v>
       </c>
       <c r="J15" t="s">
+        <v>89</v>
+      </c>
+      <c r="K15" t="s">
         <v>82</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>85</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <f t="shared" si="0"/>
         <v>0.49276649746192891</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>6458</v>
       </c>
@@ -1883,17 +1934,20 @@
         <v>79</v>
       </c>
       <c r="J16" t="s">
+        <v>89</v>
+      </c>
+      <c r="K16" t="s">
         <v>82</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>85</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <f t="shared" si="0"/>
         <v>0.87054815732424895</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>47940</v>
       </c>
@@ -1922,17 +1976,20 @@
         <v>79</v>
       </c>
       <c r="J17" t="s">
+        <v>89</v>
+      </c>
+      <c r="K17" t="s">
         <v>83</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>85</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <f t="shared" si="0"/>
         <v>0.87436378806841886</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>49841</v>
       </c>
@@ -1961,20 +2018,23 @@
         <v>79</v>
       </c>
       <c r="J18" t="s">
+        <v>89</v>
+      </c>
+      <c r="K18" t="s">
         <v>83</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>85</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <f t="shared" si="0"/>
         <v>0.53257358399711086</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>7304</v>
       </c>
@@ -2003,20 +2063,23 @@
         <v>79</v>
       </c>
       <c r="J19" t="s">
+        <v>89</v>
+      </c>
+      <c r="K19" t="s">
         <v>83</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>85</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <f t="shared" si="0"/>
         <v>0.41963307776560788</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>10301</v>
       </c>
@@ -2045,17 +2108,20 @@
         <v>79</v>
       </c>
       <c r="J20" t="s">
+        <v>89</v>
+      </c>
+      <c r="K20" t="s">
         <v>83</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>85</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <f t="shared" si="0"/>
         <v>0.89855353849140862</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>69179</v>
       </c>
@@ -2084,17 +2150,20 @@
         <v>46</v>
       </c>
       <c r="J21" t="s">
+        <v>90</v>
+      </c>
+      <c r="K21" t="s">
         <v>82</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>84</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <f t="shared" si="0"/>
         <v>0.92337269980774517</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>70391</v>
       </c>
@@ -2123,17 +2192,20 @@
         <v>46</v>
       </c>
       <c r="J22" t="s">
+        <v>90</v>
+      </c>
+      <c r="K22" t="s">
         <v>83</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>84</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <f t="shared" si="0"/>
         <v>0.95083178247219102</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>77485</v>
       </c>
@@ -2162,17 +2234,20 @@
         <v>46</v>
       </c>
       <c r="J23" t="s">
+        <v>90</v>
+      </c>
+      <c r="K23" t="s">
         <v>83</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>84</v>
       </c>
-      <c r="L23">
+      <c r="M23">
         <f t="shared" si="0"/>
         <v>0.92053945925017744</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>54709</v>
       </c>
@@ -2201,17 +2276,20 @@
         <v>46</v>
       </c>
       <c r="J24" t="s">
+        <v>90</v>
+      </c>
+      <c r="K24" t="s">
         <v>83</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>84</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <f t="shared" si="0"/>
         <v>0.87343947065382299</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>51456</v>
       </c>
@@ -2240,17 +2318,20 @@
         <v>46</v>
       </c>
       <c r="J25" t="s">
+        <v>90</v>
+      </c>
+      <c r="K25" t="s">
         <v>82</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>84</v>
       </c>
-      <c r="L25">
+      <c r="M25">
         <f t="shared" si="0"/>
         <v>0.91188588308457708</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>63598</v>
       </c>
@@ -2279,17 +2360,20 @@
         <v>46</v>
       </c>
       <c r="J26" t="s">
+        <v>90</v>
+      </c>
+      <c r="K26" t="s">
         <v>83</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>84</v>
       </c>
-      <c r="L26">
+      <c r="M26">
         <f t="shared" si="0"/>
         <v>0.89856599264127801</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>56951</v>
       </c>
@@ -2318,17 +2402,20 @@
         <v>46</v>
       </c>
       <c r="J27" t="s">
+        <v>90</v>
+      </c>
+      <c r="K27" t="s">
         <v>83</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>84</v>
       </c>
-      <c r="L27">
+      <c r="M27">
         <f t="shared" si="0"/>
         <v>0.90172253340591035</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>78000</v>
       </c>
@@ -2357,20 +2444,23 @@
         <v>46</v>
       </c>
       <c r="J28" t="s">
+        <v>90</v>
+      </c>
+      <c r="K28" t="s">
         <v>83</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>85</v>
       </c>
-      <c r="L28">
+      <c r="M28">
         <f t="shared" si="0"/>
         <v>0.91292307692307695</v>
       </c>
-      <c r="N28" t="s">
+      <c r="O28" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>44684</v>
       </c>
@@ -2399,17 +2489,20 @@
         <v>46</v>
       </c>
       <c r="J29" t="s">
+        <v>90</v>
+      </c>
+      <c r="K29" t="s">
         <v>82</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>85</v>
       </c>
-      <c r="L29">
+      <c r="M29">
         <f t="shared" si="0"/>
         <v>0.9187404887655537</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>41127</v>
       </c>
@@ -2438,20 +2531,23 @@
         <v>46</v>
       </c>
       <c r="J30" t="s">
+        <v>90</v>
+      </c>
+      <c r="K30" t="s">
         <v>83</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>84</v>
       </c>
-      <c r="L30">
+      <c r="M30">
         <f t="shared" si="0"/>
         <v>0.90142728621100499</v>
       </c>
-      <c r="N30" t="s">
+      <c r="O30" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>49016</v>
       </c>
@@ -2480,17 +2576,20 @@
         <v>46</v>
       </c>
       <c r="J31" t="s">
+        <v>90</v>
+      </c>
+      <c r="K31" t="s">
         <v>83</v>
       </c>
-      <c r="K31" t="s">
+      <c r="L31" t="s">
         <v>85</v>
       </c>
-      <c r="L31">
+      <c r="M31">
         <f t="shared" si="0"/>
         <v>0.90180757303737558</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>78137</v>
       </c>
@@ -2519,17 +2618,20 @@
         <v>46</v>
       </c>
       <c r="J32" t="s">
+        <v>90</v>
+      </c>
+      <c r="K32" t="s">
         <v>83</v>
       </c>
-      <c r="K32" t="s">
+      <c r="L32" t="s">
         <v>85</v>
       </c>
-      <c r="L32">
+      <c r="M32">
         <f t="shared" si="0"/>
         <v>0.93753279496269371</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>1599</v>
       </c>
@@ -2558,20 +2660,23 @@
         <v>58</v>
       </c>
       <c r="J33" t="s">
+        <v>58</v>
+      </c>
+      <c r="K33" t="s">
         <v>82</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
         <v>86</v>
       </c>
-      <c r="L33">
+      <c r="M33">
         <f t="shared" si="0"/>
         <v>4.3777360850531584E-2</v>
       </c>
-      <c r="M33" t="s">
+      <c r="N33" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <v>693</v>
       </c>
@@ -2600,17 +2705,20 @@
         <v>58</v>
       </c>
       <c r="J34" t="s">
+        <v>58</v>
+      </c>
+      <c r="K34" t="s">
         <v>82</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L34" t="s">
         <v>86</v>
       </c>
-      <c r="L34">
+      <c r="M34">
         <f t="shared" si="0"/>
         <v>0.24242424242424243</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>61050</v>
       </c>
@@ -2639,20 +2747,23 @@
         <v>58</v>
       </c>
       <c r="J35" t="s">
+        <v>58</v>
+      </c>
+      <c r="K35" t="s">
         <v>83</v>
       </c>
-      <c r="K35" t="s">
+      <c r="L35" t="s">
         <v>86</v>
       </c>
-      <c r="L35">
+      <c r="M35">
         <f t="shared" si="0"/>
         <v>0.61429975429975425</v>
       </c>
-      <c r="M35" t="s">
+      <c r="N35" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>61828</v>
       </c>
@@ -2681,17 +2792,20 @@
         <v>58</v>
       </c>
       <c r="J36" t="s">
+        <v>58</v>
+      </c>
+      <c r="K36" t="s">
         <v>83</v>
       </c>
-      <c r="K36" t="s">
+      <c r="L36" t="s">
         <v>86</v>
       </c>
-      <c r="L36">
+      <c r="M36">
         <f t="shared" si="0"/>
         <v>0.90627223911496413</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>45149</v>
       </c>
@@ -2720,20 +2834,23 @@
         <v>58</v>
       </c>
       <c r="J37" t="s">
+        <v>58</v>
+      </c>
+      <c r="K37" t="s">
         <v>83</v>
       </c>
-      <c r="K37" t="s">
+      <c r="L37" t="s">
         <v>86</v>
       </c>
-      <c r="L37">
+      <c r="M37">
         <f t="shared" si="0"/>
         <v>0.35635340760592704</v>
       </c>
-      <c r="M37" t="s">
+      <c r="N37" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
         <v>44180</v>
       </c>
@@ -2762,17 +2879,20 @@
         <v>58</v>
       </c>
       <c r="J38" t="s">
+        <v>58</v>
+      </c>
+      <c r="K38" t="s">
         <v>83</v>
       </c>
-      <c r="K38" t="s">
+      <c r="L38" t="s">
         <v>86</v>
       </c>
-      <c r="L38">
+      <c r="M38">
         <f t="shared" si="0"/>
         <v>0.53619284744228157</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>93770</v>
       </c>
@@ -2801,20 +2921,23 @@
         <v>58</v>
       </c>
       <c r="J39" t="s">
+        <v>58</v>
+      </c>
+      <c r="K39" t="s">
         <v>83</v>
       </c>
-      <c r="K39" t="s">
+      <c r="L39" t="s">
         <v>86</v>
       </c>
-      <c r="L39">
+      <c r="M39">
         <f t="shared" si="0"/>
         <v>0.5134904553695212</v>
       </c>
-      <c r="M39" t="s">
+      <c r="N39" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>93875</v>
       </c>
@@ -2843,19 +2966,22 @@
         <v>58</v>
       </c>
       <c r="J40" t="s">
+        <v>58</v>
+      </c>
+      <c r="K40" t="s">
         <v>83</v>
       </c>
-      <c r="K40" t="s">
+      <c r="L40" t="s">
         <v>86</v>
       </c>
-      <c r="L40">
+      <c r="M40">
         <f t="shared" si="0"/>
         <v>0.73143009320905461</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:M40" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState ref="A3:M40">
+  <autoFilter ref="A2:N40" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState ref="A3:N40">
       <sortCondition descending="1" ref="H2:H40"/>
     </sortState>
   </autoFilter>

</xml_diff>